<commit_message>
faut pas mettre de scrap dans le repo les mecs
</commit_message>
<xml_diff>
--- a/Remises/descriptionPropriete.xlsx
+++ b/Remises/descriptionPropriete.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Manipuler les trésors</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Monter l'électronique du robot sur un PCB</t>
   </si>
   <si>
-    <t>Alimenter le robot avec une batterie entre 21 et 30V</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fournir une alimentation adéquate et </t>
   </si>
   <si>
@@ -204,6 +201,12 @@
   </si>
   <si>
     <t>Alimenter adéquatement chaque élément du système</t>
+  </si>
+  <si>
+    <t>Alimenter le robot avec une batterie</t>
+  </si>
+  <si>
+    <t>Tension entre 21V et 30V</t>
   </si>
 </sst>
 </file>
@@ -536,11 +539,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,21 +558,6 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -612,6 +597,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AG18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C1:AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,842 +913,849 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22" t="s">
+      <c r="D1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="32"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="9" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="33"/>
+      <c r="T1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="10"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="11"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="33"/>
     </row>
     <row r="2" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="D2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="13"/>
+      <c r="D2" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="36"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
     </row>
     <row r="3" spans="3:33" ht="380.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="G3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" s="14" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="T3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="U3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="6" t="s">
+      <c r="V3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AB3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD3" s="14" t="s">
+      <c r="AC3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AF3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AG3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="32">
-        <v>5</v>
-      </c>
-      <c r="P4" s="33">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="34">
-        <v>5</v>
-      </c>
-      <c r="R4" s="32">
-        <v>5</v>
-      </c>
-      <c r="S4" s="34">
-        <v>5</v>
-      </c>
-      <c r="T4" s="32">
-        <v>5</v>
-      </c>
-      <c r="U4" s="33">
-        <v>5</v>
-      </c>
-      <c r="V4" s="34">
-        <v>5</v>
-      </c>
-      <c r="W4" s="32"/>
-      <c r="X4" s="33">
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="26">
+        <v>5</v>
+      </c>
+      <c r="P4" s="27">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>5</v>
+      </c>
+      <c r="R4" s="26">
+        <v>5</v>
+      </c>
+      <c r="S4" s="28">
+        <v>5</v>
+      </c>
+      <c r="T4" s="26">
+        <v>5</v>
+      </c>
+      <c r="U4" s="27">
+        <v>5</v>
+      </c>
+      <c r="V4" s="28">
+        <v>5</v>
+      </c>
+      <c r="W4" s="26"/>
+      <c r="X4" s="27">
         <v>2</v>
       </c>
-      <c r="Y4" s="34">
-        <v>5</v>
-      </c>
-      <c r="Z4" s="32">
+      <c r="Y4" s="28">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="26">
         <v>1</v>
       </c>
-      <c r="AA4" s="33">
+      <c r="AA4" s="27">
         <v>1</v>
       </c>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="34"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="27"/>
+      <c r="AF4" s="27"/>
+      <c r="AG4" s="28"/>
     </row>
     <row r="5" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="16">
-        <v>5</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="D5" s="10">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="8">
-        <v>5</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="G5" s="7">
+        <v>5</v>
+      </c>
+      <c r="H5" s="11">
         <v>4</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="16">
+      <c r="I5" s="10"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="10">
         <v>4</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="7">
         <v>3</v>
       </c>
-      <c r="Y5" s="17">
+      <c r="Y5" s="11">
         <v>4</v>
       </c>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="17"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="11"/>
     </row>
     <row r="6" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="16">
-        <v>5</v>
-      </c>
-      <c r="P6" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="17">
-        <v>5</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="17"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="10">
+        <v>5</v>
+      </c>
+      <c r="P6" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>5</v>
+      </c>
+      <c r="R6" s="10"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="11"/>
     </row>
     <row r="7" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="17">
-        <v>5</v>
-      </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="17"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>5</v>
+      </c>
+      <c r="R7" s="10"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="11"/>
     </row>
     <row r="8" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="17"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="8">
-        <v>5</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>5</v>
-      </c>
-      <c r="AG8" s="17">
+      <c r="D8" s="10"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="7">
+        <v>5</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>5</v>
+      </c>
+      <c r="AG8" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="17">
-        <v>5</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="17"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="17"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="11">
+        <v>5</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="11"/>
     </row>
     <row r="10" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8">
-        <v>5</v>
-      </c>
-      <c r="H10" s="17">
-        <v>5</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="17"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="17"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <v>5</v>
+      </c>
+      <c r="H10" s="11">
+        <v>5</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="11"/>
     </row>
     <row r="11" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="10">
         <v>4</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="17">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="11">
         <v>2</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="8">
+      <c r="I11" s="10"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="7">
         <v>3</v>
       </c>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="17"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="11"/>
     </row>
     <row r="12" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="8">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="8">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="17"/>
-      <c r="Z12" s="16">
-        <v>5</v>
-      </c>
-      <c r="AA12" s="8">
-        <v>5</v>
-      </c>
-      <c r="AB12" s="8">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="17">
+      <c r="D12" s="10"/>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="7">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="10">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="11">
         <v>1</v>
       </c>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="8"/>
-      <c r="AF12" s="8"/>
-      <c r="AG12" s="17"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="11"/>
     </row>
     <row r="13" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="16">
+      <c r="D13" s="10"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10">
         <v>2</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="16">
+      <c r="J13" s="7"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="10">
         <v>4</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>3</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="11">
         <v>4</v>
       </c>
-      <c r="R13" s="16"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="16">
+      <c r="R13" s="10"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="10">
         <v>3</v>
       </c>
-      <c r="U13" s="8">
+      <c r="U13" s="7">
         <v>3</v>
       </c>
-      <c r="V13" s="17">
+      <c r="V13" s="11">
         <v>3</v>
       </c>
-      <c r="W13" s="16"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="17"/>
-      <c r="AD13" s="16"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="17"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="11"/>
     </row>
     <row r="14" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8">
-        <v>5</v>
-      </c>
-      <c r="AC14" s="17"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="8">
-        <v>5</v>
-      </c>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="17"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="7">
+        <v>5</v>
+      </c>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="11"/>
     </row>
     <row r="15" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="10">
         <v>1</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>2</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>2</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="11">
         <v>1</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="10">
         <v>1</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>2</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="11">
         <v>2</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="10">
         <v>2</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="7">
         <v>2</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="11">
         <v>2</v>
       </c>
-      <c r="O15" s="16">
-        <v>5</v>
-      </c>
-      <c r="P15" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q15" s="17">
-        <v>5</v>
-      </c>
-      <c r="R15" s="16">
+      <c r="O15" s="10">
+        <v>5</v>
+      </c>
+      <c r="P15" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>5</v>
+      </c>
+      <c r="R15" s="10">
         <v>4</v>
       </c>
-      <c r="S15" s="17">
+      <c r="S15" s="11">
         <v>4</v>
       </c>
-      <c r="T15" s="16">
+      <c r="T15" s="10">
         <v>4</v>
       </c>
-      <c r="U15" s="8">
+      <c r="U15" s="7">
         <v>4</v>
       </c>
-      <c r="V15" s="17">
+      <c r="V15" s="11">
         <v>4</v>
       </c>
-      <c r="W15" s="16">
+      <c r="W15" s="10">
         <v>3</v>
       </c>
-      <c r="X15" s="8">
+      <c r="X15" s="7">
         <v>3</v>
       </c>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="17"/>
-      <c r="AD15" s="16"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="17"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="11"/>
     </row>
     <row r="16" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="16">
-        <v>5</v>
-      </c>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="17"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="8">
-        <v>5</v>
-      </c>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="17"/>
-      <c r="AD16" s="16"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="17"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="10">
+        <v>5</v>
+      </c>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="11"/>
     </row>
     <row r="17" spans="3:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="12">
         <v>4</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13">
         <v>4</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="13">
         <v>3</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="14">
         <v>4</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="19"/>
-      <c r="AF17" s="19"/>
-      <c r="AG17" s="20"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="14"/>
     </row>
-    <row r="18" spans="3:33" ht="79.5" x14ac:dyDescent="0.25">
-      <c r="M18" s="4" t="s">
-        <v>36</v>
+    <row r="18" spans="3:33" ht="123" x14ac:dyDescent="0.25">
+      <c r="D18" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD1:AG1"/>
@@ -1752,10 +1765,6 @@
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>